<commit_message>
Hail revB production files
</commit_message>
<xml_diff>
--- a/hardware/hail/rev_b/hail_bom.xlsx
+++ b/hardware/hail/rev_b/hail_bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="hail_bom" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="154">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -43,10 +43,19 @@
     <t xml:space="preserve">DIGIKEY</t>
   </si>
   <si>
+    <t xml:space="preserve">MOUSER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEWARK</t>
+  </si>
+  <si>
     <t xml:space="preserve">RICHARDSON_RFPD</t>
   </si>
   <si>
-    <t xml:space="preserve">Already In Lab</t>
+    <t xml:space="preserve">TP_SIGNAL_NAME</t>
   </si>
   <si>
     <t xml:space="preserve">FRACTUS-2.4GHZ-FR05-S1-N-0-110</t>
@@ -64,9 +73,6 @@
     <t xml:space="preserve">FR05-S1-N-0110B</t>
   </si>
   <si>
-    <t xml:space="preserve">PowerBlade Supplies</t>
-  </si>
-  <si>
     <t xml:space="preserve">BAL-NRF01D3</t>
   </si>
   <si>
@@ -79,7 +85,7 @@
     <t xml:space="preserve">497-13637-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve"> ICs Box</t>
+    <t xml:space="preserve">511-BAL-NRF01D3</t>
   </si>
   <si>
     <t xml:space="preserve">1.5pF</t>
@@ -187,9 +193,6 @@
     <t xml:space="preserve">67-2125-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Signpost Controller</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.5k</t>
   </si>
   <si>
@@ -199,9 +202,6 @@
     <t xml:space="preserve">FB1</t>
   </si>
   <si>
-    <t xml:space="preserve">0402 Ferrite Bead</t>
-  </si>
-  <si>
     <t xml:space="preserve">1276-6395-1-ND</t>
   </si>
   <si>
@@ -220,28 +220,34 @@
     <t xml:space="preserve">H125274CT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">M12PTH-CST-L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1X12-CASTELLATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1011E-12-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M12PTH-CST-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J3</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC2030-JLINK-NL_NOSILK</t>
   </si>
   <si>
     <t xml:space="preserve">TC2030-IDC-NL_NOSILK</t>
   </si>
   <si>
-    <t xml:space="preserve">J2, J3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M12PTH-CST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1X12-CASTELLATED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JP3, JP4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Header 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S1011E-12-ND</t>
+    <t xml:space="preserve">J4, J5</t>
   </si>
   <si>
     <t xml:space="preserve">6.8nH</t>
@@ -283,7 +289,7 @@
     <t xml:space="preserve">0402_RES</t>
   </si>
   <si>
-    <t xml:space="preserve">R1, R2, R3, R4, R5</t>
+    <t xml:space="preserve">R1, R2, R3, R4, R5, R6</t>
   </si>
   <si>
     <t xml:space="preserve">Resistor</t>
@@ -295,7 +301,7 @@
     <t xml:space="preserve">10k</t>
   </si>
   <si>
-    <t xml:space="preserve">R6, R7, R8, R9</t>
+    <t xml:space="preserve">R7, R8, R9, R10</t>
   </si>
   <si>
     <t xml:space="preserve">1276-3431-1-ND</t>
@@ -304,7 +310,7 @@
     <t xml:space="preserve">100k</t>
   </si>
   <si>
-    <t xml:space="preserve">R10, R11, R12</t>
+    <t xml:space="preserve">R11, R12, R13</t>
   </si>
   <si>
     <t xml:space="preserve">1276-3432-1-ND</t>
@@ -322,6 +328,18 @@
     <t xml:space="preserve">SW1020CT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">TPB1,27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1,27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test pad</t>
+  </si>
+  <si>
     <t xml:space="preserve">FT231XQ</t>
   </si>
   <si>
@@ -337,6 +355,9 @@
     <t xml:space="preserve">768-1128-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">FT231XQ-R</t>
+  </si>
+  <si>
     <t xml:space="preserve">FXOS8700CQ</t>
   </si>
   <si>
@@ -352,6 +373,9 @@
     <t xml:space="preserve">FXOS8700CQR1CT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">FXOS8700CQR1</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISL29035</t>
   </si>
   <si>
@@ -367,6 +391,9 @@
     <t xml:space="preserve">ISL29035IROZ-T7CT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">ISL29035IROZ-T7</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAX8887EZK33+T</t>
   </si>
   <si>
@@ -382,9 +409,6 @@
     <t xml:space="preserve">MAX8887EZK33+TCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Signpost RF Spectrum</t>
-  </si>
-  <si>
     <t xml:space="preserve">NRF51822QF</t>
   </si>
   <si>
@@ -400,9 +424,6 @@
     <t xml:space="preserve">1490-1049-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">ICs Box</t>
-  </si>
-  <si>
     <t xml:space="preserve">SAM4LC8BA</t>
   </si>
   <si>
@@ -446,9 +467,6 @@
   </si>
   <si>
     <t xml:space="preserve">887-2003-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Parts Box</t>
   </si>
   <si>
     <t xml:space="preserve">FH1600015</t>
@@ -473,7 +491,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -494,13 +512,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -545,16 +556,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -573,29 +576,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="30.9132653061224"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.6683673469388"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="54.8061224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -623,316 +628,316 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="G5" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="E9" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="E10" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="E14" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="0" t="s">
         <v>59</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>1</v>
       </c>
@@ -955,9 +960,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>66</v>
@@ -971,388 +976,431 @@
       <c r="E16" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="F16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="G17" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="C18" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="0" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="C19" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="D19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="F19" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="0" t="s">
+      <c r="G19" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="0" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="C20" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="E20" s="0" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B20" s="0" t="s">
+      <c r="F20" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="G20" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="0" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="F21" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B22" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="G22" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="E23" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="0" t="s">
+      <c r="B24" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="C24" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B24" s="0" t="s">
+      <c r="F24" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="0" t="s">
+      <c r="G24" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="0" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="C25" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B25" s="0" t="s">
+      <c r="F25" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" s="0" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="C26" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="E26" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="F26" s="0" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" s="0" t="s">
+      <c r="G26" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="0" t="s">
+      <c r="I26" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E26" s="0" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="C27" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="E27" s="0" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B27" s="0" t="s">
+      <c r="F27" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="0" t="s">
+      <c r="G27" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="I27" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="F27" s="0" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="C28" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="E28" s="0" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" s="0" t="s">
+      <c r="F28" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" s="0" t="s">
+      <c r="G28" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="I28" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="0" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="C29" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="E29" s="0" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="F29" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D29" s="0" t="s">
+      <c r="G29" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="E29" s="0" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="C30" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="E30" s="0" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B30" s="0" t="s">
+      <c r="F30" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D30" s="0" t="s">
+      <c r="G30" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="E30" s="0" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="C31" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="E31" s="0" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" s="0" t="s">
+      <c r="F31" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="G31" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E31" s="0" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="C32" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="E32" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="F32" s="0" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="C32" s="0" t="s">
+      <c r="G32" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="D32" s="0" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="C33" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="D33" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="G32" s="0" t="s">
+      <c r="F33" s="0" t="s">
         <v>147</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>